<commit_message>
Criação de Arquivos Básicos e Modificações na Documentação
</commit_message>
<xml_diff>
--- a/documentacao/backlog.xlsx
+++ b/documentacao/backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzo_reis\Documents\Enzo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzo_reis\Documents\Enzo\formula1_novo\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
   <si>
     <t>identificar os requisitos funcionais - funções principais do jogo</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>Inicialização do Projeto</t>
+  </si>
+  <si>
+    <t>index.html(front)</t>
+  </si>
+  <si>
+    <t>style.css(front)</t>
+  </si>
+  <si>
+    <t>f1_main.js(back)</t>
+  </si>
+  <si>
+    <t>f1_class.js(back)</t>
   </si>
 </sst>
 </file>
@@ -276,15 +288,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -292,11 +310,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -337,10 +370,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G27"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,265 +1131,445 @@
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="C15" s="17"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
+      <c r="C18" s="17"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
+      <c r="C19" s="17"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="C26" s="17"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
+  <mergeCells count="31">
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B17:C17"/>
@@ -1360,6 +1579,11 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>